<commit_message>
Excel code and TestNg Annotation added
</commit_message>
<xml_diff>
--- a/jenkinTest/GoogleSearch.xlsx
+++ b/jenkinTest/GoogleSearch.xlsx
@@ -1,47 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\valmiki\Selenium program New\jenkinTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valmiki\git\UAT\jenkinTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9630"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Topic to search</t>
+    <t>Username</t>
   </si>
   <si>
-    <t>Intelegain</t>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Valmiki.k@intelegain.com</t>
+  </si>
+  <si>
+    <t>Test@123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -49,7 +50,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -76,14 +84,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -142,7 +155,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -177,7 +190,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -352,39 +365,43 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>